<commit_message>
divided profile into 4 parts
</commit_message>
<xml_diff>
--- a/summer2021.xlsx
+++ b/summer2021.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="101">
   <si>
     <t>Task</t>
   </si>
@@ -317,6 +317,18 @@
   </si>
   <si>
     <t>(login)</t>
+  </si>
+  <si>
+    <t>suggestion card</t>
+  </si>
+  <si>
+    <t>(cards)</t>
+  </si>
+  <si>
+    <t>desgin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code </t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1192,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1190,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" activeCellId="1" sqref="I22 F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="18"/>
@@ -2729,14 +2741,26 @@
         <v>42</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="J22" s="3" t="s">
         <v>26</v>
       </c>

</xml_diff>